<commit_message>
data-ta.xlsx added missing rows, validated html files for xhtml
</commit_message>
<xml_diff>
--- a/g2-04-taplan/data-ta.xlsx
+++ b/g2-04-taplan/data-ta.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessakomar/Documents/Graz/2nd Semester/HCI/HCI/taplan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Megaport\Desktop\HCI23\HCI\g2-04-taplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF434C8-6EA4-B04F-9DC1-F48F53ED4A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEB3197-2990-4558-BA79-716E4B98CCD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1520" windowWidth="19200" windowHeight="21100" tabRatio="503" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="3330" windowWidth="38400" windowHeight="15060" tabRatio="503" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Background Q" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="145">
   <si>
     <t>Browser</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Connection</t>
   </si>
   <si>
-    <t>Newspaper Archive</t>
-  </si>
-  <si>
-    <t>defacto.at</t>
-  </si>
-  <si>
     <t>Previous Usability Tests</t>
   </si>
   <si>
@@ -207,18 +201,6 @@
     <t>Contradictory information "free delivery" or "free delivery above 200,- EUR"</t>
   </si>
   <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>CT</t>
-  </si>
-  <si>
-    <t>TG</t>
-  </si>
-  <si>
-    <t>SS</t>
-  </si>
-  <si>
     <t>Unsure which catalogue, since no name is displayed.</t>
   </si>
   <si>
@@ -318,9 +300,6 @@
     <t>12 Return Visit</t>
   </si>
   <si>
-    <t>14 ??</t>
-  </si>
-  <si>
     <t>General Information</t>
   </si>
   <si>
@@ -408,9 +387,6 @@
     <t>13 Likely to Recommend</t>
   </si>
   <si>
-    <t>15 ??</t>
-  </si>
-  <si>
     <t>man</t>
   </si>
   <si>
@@ -469,6 +445,33 @@
   </si>
   <si>
     <t>"Michael"</t>
+  </si>
+  <si>
+    <t>KS</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>VK</t>
+  </si>
+  <si>
+    <t>Lives in Graz</t>
+  </si>
+  <si>
+    <t>Visited website</t>
+  </si>
+  <si>
+    <t>Visited Pharmacy</t>
+  </si>
+  <si>
+    <t>14 Likely to Order</t>
+  </si>
+  <si>
+    <t>15 Likely Consultation</t>
   </si>
 </sst>
 </file>
@@ -959,7 +962,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1071,9 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1090,12 +1090,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1111,7 +1116,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1431,58 +1436,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB13"/>
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="168" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="U1" zoomScale="168" workbookViewId="0">
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" customWidth="1"/>
-    <col min="14" max="14" width="6.33203125" customWidth="1"/>
-    <col min="15" max="15" width="7.1640625" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" customWidth="1"/>
-    <col min="17" max="17" width="6.33203125" customWidth="1"/>
-    <col min="18" max="18" width="7.6640625" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" customWidth="1"/>
-    <col min="20" max="20" width="13.33203125" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.85546875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.28515625" customWidth="1"/>
+    <col min="18" max="18" width="7.7109375" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
+    <col min="20" max="20" width="13.28515625" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
-    <col min="23" max="23" width="17.1640625" customWidth="1"/>
-    <col min="24" max="24" width="20.83203125" customWidth="1"/>
-    <col min="25" max="25" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13.83203125" customWidth="1"/>
-    <col min="27" max="27" width="13.1640625" customWidth="1"/>
-    <col min="28" max="28" width="22.33203125" customWidth="1"/>
+    <col min="23" max="23" width="17.140625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" customWidth="1"/>
+    <col min="27" max="27" width="13.85546875" customWidth="1"/>
+    <col min="28" max="28" width="13.140625" customWidth="1"/>
+    <col min="29" max="29" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="1:28" s="6" customFormat="1" x14ac:dyDescent="0.15">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C3" s="11" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="11" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G3" s="13"/>
       <c r="H3" s="11" t="s">
@@ -1490,46 +1496,47 @@
       </c>
       <c r="I3" s="13"/>
       <c r="J3" s="11" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="11" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="N3" s="12"/>
       <c r="O3" s="12"/>
       <c r="P3" s="11" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="12"/>
       <c r="R3" s="12"/>
       <c r="S3" s="11" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
       <c r="V3" s="12"/>
       <c r="W3" s="13"/>
       <c r="X3" s="74" t="s">
-        <v>112</v>
-      </c>
-      <c r="Y3" s="75"/>
-      <c r="Z3" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA3" s="75"/>
-      <c r="AB3" s="13"/>
-    </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="77"/>
+      <c r="AA3" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB3" s="75"/>
+      <c r="AC3" s="13"/>
+    </row>
+    <row r="4" spans="1:29" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>8</v>
@@ -1541,10 +1548,10 @@
         <v>10</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>12</v>
@@ -1553,34 +1560,34 @@
         <v>13</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="M4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="O4" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="P4" s="14" t="s">
         <v>13</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="S4" s="16" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="T4" s="16" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="U4" s="16" t="s">
         <v>14</v>
@@ -1589,33 +1596,36 @@
         <v>0</v>
       </c>
       <c r="W4" s="17" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>16</v>
+        <v>141</v>
       </c>
       <c r="Z4" s="16" t="s">
-        <v>113</v>
+        <v>142</v>
       </c>
       <c r="AA4" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="AB4" s="17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.15">
+        <v>106</v>
+      </c>
+      <c r="AB4" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC4" s="17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D5" s="58">
         <v>22</v>
@@ -1643,16 +1653,17 @@
       <c r="Z5" s="49"/>
       <c r="AA5" s="49"/>
       <c r="AB5" s="49"/>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC5" s="49"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>140</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>124</v>
+        <v>132</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>116</v>
       </c>
       <c r="D6" s="58">
         <v>21</v>
@@ -1677,19 +1688,20 @@
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
-      <c r="Z6" s="49"/>
-      <c r="AA6" s="4"/>
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="49"/>
       <c r="AB6" s="4"/>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC6" s="4"/>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D7" s="58">
         <v>21</v>
@@ -1714,19 +1726,20 @@
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
-      <c r="Z7" s="49"/>
-      <c r="AA7" s="4"/>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="49"/>
       <c r="AB7" s="4"/>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC7" s="4"/>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D8" s="58">
         <v>18</v>
@@ -1751,26 +1764,27 @@
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
-      <c r="Z8" s="49"/>
-      <c r="AA8" s="4"/>
+      <c r="Z8" s="4"/>
+      <c r="AA8" s="49"/>
       <c r="AB8" s="4"/>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.15">
+      <c r="AC8" s="4"/>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>143</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="71" t="s">
+        <v>135</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D9" s="59">
         <v>21</v>
       </c>
       <c r="E9" s="24"/>
       <c r="F9" s="24"/>
-      <c r="G9" s="70"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="24"/>
       <c r="I9" s="24"/>
       <c r="J9" s="26"/>
@@ -1789,11 +1803,12 @@
       <c r="W9" s="24"/>
       <c r="X9" s="24"/>
       <c r="Y9" s="24"/>
-      <c r="Z9" s="71"/>
-      <c r="AA9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="70"/>
       <c r="AB9" s="24"/>
-    </row>
-    <row r="10" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="AC9" s="24"/>
+    </row>
+    <row r="10" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="K10" s="22"/>
       <c r="L10" s="22"/>
       <c r="N10" s="22"/>
@@ -1801,10 +1816,10 @@
       <c r="Q10" s="22"/>
       <c r="R10" s="22"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C11" s="5"/>
       <c r="D11" s="57"/>
@@ -1814,7 +1829,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
       <c r="J11" s="46" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="K11" s="51" t="e">
         <f>AVERAGE(K5:K9)</f>
@@ -1825,7 +1840,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M11" s="46" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="N11" s="51" t="e">
         <f>AVERAGE(N5:N9)</f>
@@ -1836,7 +1851,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P11" s="46" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="51" t="e">
         <f>AVERAGE(Q5:Q9)</f>
@@ -1853,22 +1868,22 @@
       <c r="T11" s="20"/>
       <c r="U11" s="20"/>
       <c r="V11" s="46" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="W11" s="51" t="e">
         <f>AVERAGE(W5:W9)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="29"/>
       <c r="B12" s="31" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="5"/>
       <c r="D12" s="33"/>
       <c r="J12" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="K12" s="33" t="e">
         <f>MEDIAN(K5:K9)</f>
@@ -1879,7 +1894,7 @@
         <v>#NUM!</v>
       </c>
       <c r="M12" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="N12" s="33" t="e">
         <f>MEDIAN(N5:N9)</f>
@@ -1890,7 +1905,7 @@
         <v>#NUM!</v>
       </c>
       <c r="P12" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="Q12" s="33" t="e">
         <f>MEDIAN(Q5:Q9)</f>
@@ -1905,28 +1920,28 @@
         <v>#NUM!</v>
       </c>
       <c r="V12" s="46" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="W12" s="33" t="e">
         <f>MEDIAN(W5:W9)</f>
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="J13" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="M13" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="V13" s="46" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="Z3:AA3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="X3:Z3"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
@@ -1943,22 +1958,22 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="7" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" s="40" t="s">
         <v>5</v>
       </c>
@@ -1967,104 +1982,104 @@
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="32">
+        <v>1</v>
+      </c>
+      <c r="D5" s="32">
+        <v>1</v>
+      </c>
+      <c r="E5" s="32">
+        <v>1</v>
+      </c>
+      <c r="F5" s="32">
+        <v>1</v>
+      </c>
+      <c r="G5" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="32">
+        <v>1</v>
+      </c>
+      <c r="D6" s="32">
+        <v>1</v>
+      </c>
+      <c r="E6" s="32">
+        <v>1</v>
+      </c>
+      <c r="F6" s="32">
+        <v>1</v>
+      </c>
+      <c r="G6" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="43" t="s">
-        <v>126</v>
-      </c>
-      <c r="C5" s="32">
-        <v>1</v>
-      </c>
-      <c r="D5" s="32">
-        <v>1</v>
-      </c>
-      <c r="E5" s="32">
-        <v>1</v>
-      </c>
-      <c r="F5" s="32">
-        <v>1</v>
-      </c>
-      <c r="G5" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="B7" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="32">
+        <v>1</v>
+      </c>
+      <c r="D7" s="32">
+        <v>1</v>
+      </c>
+      <c r="E7" s="32">
+        <v>1</v>
+      </c>
+      <c r="F7" s="32">
+        <v>1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="43" t="s">
-        <v>127</v>
-      </c>
-      <c r="C6" s="32">
-        <v>1</v>
-      </c>
-      <c r="D6" s="32">
-        <v>1</v>
-      </c>
-      <c r="E6" s="32">
-        <v>1</v>
-      </c>
-      <c r="F6" s="32">
-        <v>1</v>
-      </c>
-      <c r="G6" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" s="32">
-        <v>1</v>
-      </c>
-      <c r="D7" s="32">
-        <v>1</v>
-      </c>
-      <c r="E7" s="32">
-        <v>1</v>
-      </c>
-      <c r="F7" s="32">
-        <v>1</v>
-      </c>
-      <c r="G7" s="32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="B8" s="43" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C8" s="32">
         <v>1</v>
@@ -2082,12 +2097,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="72" t="s">
-        <v>130</v>
+        <v>23</v>
+      </c>
+      <c r="B9" s="71" t="s">
+        <v>122</v>
       </c>
       <c r="C9" s="32">
         <v>1</v>
@@ -2105,7 +2120,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29"/>
       <c r="B10" s="29" t="s">
         <v>1</v>
@@ -2131,7 +2146,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="29"/>
       <c r="B11" s="29" t="s">
         <v>2</v>
@@ -2170,84 +2185,84 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="36.1640625" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="10" width="4.6640625" style="61" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" style="61" customWidth="1"/>
+    <col min="7" max="10" width="4.7109375" style="61" customWidth="1"/>
+    <col min="11" max="11" width="6.140625" style="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="G3" s="66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G3" s="65" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="62" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="67" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="62" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="C4" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="D4" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="F4" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>41</v>
-      </c>
       <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" t="s">
         <v>55</v>
       </c>
-      <c r="D5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E5" t="s">
-        <v>61</v>
-      </c>
       <c r="F5" s="48" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="G5" s="61">
         <v>2</v>
@@ -2266,25 +2281,25 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>SUM(A5,1)</f>
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F6" s="48" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G6" s="61">
         <v>3</v>
@@ -2303,25 +2318,25 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>SUM(A6,1)</f>
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" t="s">
         <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E7" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
       </c>
       <c r="G7" s="61">
         <v>4</v>
@@ -2340,25 +2355,25 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>SUM(A7,1)</f>
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G8" s="61">
         <v>3</v>
@@ -2377,25 +2392,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>SUM(A8,1)</f>
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="F9" s="48" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="G9" s="61">
         <v>3</v>
@@ -2414,24 +2429,24 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F10" s="48" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="G10" s="61">
         <v>2</v>
@@ -2450,24 +2465,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" t="s">
         <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
       </c>
       <c r="G11" s="61">
         <v>2</v>
@@ -2486,24 +2501,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12" s="69" t="s">
-        <v>77</v>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="68" t="s">
+        <v>71</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D12" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E12" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F12" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G12" s="61">
         <v>2</v>
@@ -2522,24 +2537,24 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13" s="69" t="s">
-        <v>77</v>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="68" t="s">
+        <v>71</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D13" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E13" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" s="48" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G13" s="61">
         <v>2</v>
@@ -2558,24 +2573,24 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
       <c r="D14" s="48" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="G14" s="61">
         <v>1</v>
@@ -2608,84 +2623,84 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="36" customWidth="1"/>
-    <col min="3" max="3" width="35.1640625" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" customWidth="1"/>
-    <col min="5" max="5" width="26.1640625" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
-    <col min="7" max="10" width="4.6640625" style="61" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" style="61" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.140625" customWidth="1"/>
+    <col min="7" max="10" width="4.7109375" style="61" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" style="61" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="G3" s="66" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="62" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G3" s="65" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="62" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="67" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="67" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="D4" s="67" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="67" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="68" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>116</v>
-      </c>
-      <c r="E4" s="68" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="65" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="67" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="F4" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="73" t="s">
+        <v>136</v>
+      </c>
+      <c r="H4" s="73" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="J4" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" s="66" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E5" s="48" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F5" s="48" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="G5" s="61">
         <v>2</v>
@@ -2704,25 +2719,25 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <f>SUM(A5,1)</f>
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F6" s="48" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G6" s="61">
         <v>3</v>
@@ -2741,25 +2756,25 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <f>SUM(A6,1)</f>
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G7" s="61">
         <v>4</v>
@@ -2778,25 +2793,25 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <f>SUM(A7,1)</f>
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G8" s="61">
         <v>3</v>
@@ -2815,25 +2830,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <f>SUM(A8,1)</f>
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G9" s="61">
         <v>3</v>
@@ -2852,24 +2867,24 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F10" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G10" s="61">
         <v>2</v>
@@ -2888,24 +2903,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G11" s="61">
         <v>2</v>
@@ -2924,24 +2939,24 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G12" s="61">
         <v>2</v>
@@ -2960,24 +2975,24 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G13" s="61">
         <v>2</v>
@@ -2996,24 +3011,24 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G14" s="61">
         <v>1</v>
@@ -3042,108 +3057,108 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" style="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.33203125" customWidth="1"/>
-    <col min="16" max="17" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.28515625" customWidth="1"/>
+    <col min="16" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.140625" customWidth="1"/>
     <col min="19" max="19" width="22" customWidth="1"/>
-    <col min="20" max="20" width="15.6640625" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" customWidth="1"/>
+    <col min="22" max="22" width="17.7109375" customWidth="1"/>
     <col min="23" max="23" width="16" customWidth="1"/>
     <col min="24" max="24" width="25" customWidth="1"/>
-    <col min="25" max="25" width="19.83203125" customWidth="1"/>
-    <col min="26" max="26" width="10.1640625" customWidth="1"/>
-    <col min="27" max="27" width="7.83203125" customWidth="1"/>
-    <col min="28" max="28" width="8.6640625" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" customWidth="1"/>
-    <col min="30" max="30" width="8.6640625" customWidth="1"/>
-    <col min="31" max="31" width="29.33203125" customWidth="1"/>
+    <col min="25" max="25" width="19.85546875" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" customWidth="1"/>
+    <col min="27" max="27" width="7.85546875" customWidth="1"/>
+    <col min="28" max="28" width="8.7109375" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" customWidth="1"/>
+    <col min="31" max="31" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="34" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="G3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="H3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="I3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="J3" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="K3" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="35" t="s">
-        <v>35</v>
-      </c>
       <c r="L3" s="35" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="M3" s="35" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="O3" s="16" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>93</v>
+        <v>143</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.15">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="43" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C4" s="37">
         <v>5</v>
@@ -3191,12 +3206,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C5" s="37">
         <v>4</v>
@@ -3244,12 +3259,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B6" s="43" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C6" s="37">
         <v>3</v>
@@ -3297,12 +3312,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C7" s="37">
         <v>2</v>
@@ -3350,12 +3365,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="22" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="72" t="s">
-        <v>130</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="71" t="s">
+        <v>122</v>
       </c>
       <c r="C8" s="38">
         <v>3</v>
@@ -3403,7 +3418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
@@ -3416,10 +3431,10 @@
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
     </row>
-    <row r="10" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:17" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="29"/>
       <c r="B10" s="29" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C10" s="56">
         <f>AVERAGE(C4:C8)</f>
@@ -3482,7 +3497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="22" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" s="22" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29"/>
       <c r="B11" s="29" t="s">
         <v>6</v>

</xml_diff>